<commit_message>
romain maj avec photos
</commit_message>
<xml_diff>
--- a/Rapport_detecteur_tonalite.xlsx
+++ b/Rapport_detecteur_tonalite.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sesa466660\Documents\Projet_frelons\Projet-frelons\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D7825B1A-67B5-482E-A6BB-D7281BBA71F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE651A4B-9856-43F1-A831-47301C94ED08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{17A6E8DD-4580-4AEB-8DB9-002E238FFB9C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Résumé" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>Carte avec micro d'origine + R2 = 220 Ohms et C1 = 4.7µF</t>
   </si>
@@ -237,14 +237,56 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -252,47 +294,14 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -355,6 +364,138 @@
         <a:xfrm>
           <a:off x="7410450" y="647700"/>
           <a:ext cx="7457143" cy="4904762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>18000</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>113769</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Image 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A26A5B45-6050-4C3A-8507-F2A256463720}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="6534150"/>
+          <a:ext cx="8933400" cy="4685769"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>37220</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>113668</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Image 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{980E5D3F-40B9-441B-AD1E-0C65AA7CD81D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="390525" y="12068175"/>
+          <a:ext cx="7038095" cy="5057143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>122952</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>180262</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Image 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A8D9D30-EC97-4893-BD78-B9C3AF11959F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8153400" y="12058650"/>
+          <a:ext cx="6980952" cy="5704762"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -663,10 +804,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31DACCDA-234F-438F-A31F-18790C0A2430}">
-  <dimension ref="A1:O26"/>
+  <dimension ref="A1:R60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:N1"/>
+      <selection activeCell="L59" sqref="L59:R60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -675,335 +816,377 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2"/>
-      <c r="B1" s="3" t="s">
+      <c r="A1" s="1"/>
+      <c r="B1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="4" t="s">
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="9" t="s">
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="7"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="2"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="6" t="s">
+      <c r="A2" s="1"/>
+      <c r="B2" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="5" t="s">
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1" t="s">
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
     </row>
     <row r="6" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="11" t="s">
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="13"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="9"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="15"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="12"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="18"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="15"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10" t="s">
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
+      <c r="A11" s="4"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1" t="s">
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
     </row>
     <row r="15" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
-      <c r="I15" s="19"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="19"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="19"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="19"/>
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="19"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="19"/>
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="19"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="19"/>
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="19"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="19"/>
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="19"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="19"/>
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="19"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="19"/>
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="19"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="19"/>
-      <c r="I24" s="19"/>
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="19"/>
-      <c r="B25" s="19"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="19"/>
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="19"/>
-      <c r="B26" s="19"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19"/>
-      <c r="I26" s="19"/>
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+    </row>
+    <row r="59" spans="2:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C59" s="21"/>
+      <c r="D59" s="21"/>
+      <c r="E59" s="21"/>
+      <c r="F59" s="21"/>
+      <c r="G59" s="21"/>
+      <c r="H59" s="21"/>
+      <c r="I59" s="21"/>
+      <c r="L59" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="M59" s="20"/>
+      <c r="N59" s="20"/>
+      <c r="O59" s="20"/>
+      <c r="P59" s="20"/>
+      <c r="Q59" s="20"/>
+      <c r="R59" s="20"/>
+    </row>
+    <row r="60" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B60" s="22"/>
+      <c r="C60" s="22"/>
+      <c r="D60" s="22"/>
+      <c r="E60" s="22"/>
+      <c r="F60" s="22"/>
+      <c r="G60" s="22"/>
+      <c r="H60" s="22"/>
+      <c r="I60" s="22"/>
+      <c r="L60" s="20"/>
+      <c r="M60" s="20"/>
+      <c r="N60" s="20"/>
+      <c r="O60" s="20"/>
+      <c r="P60" s="20"/>
+      <c r="Q60" s="20"/>
+      <c r="R60" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="20">
+    <mergeCell ref="F3:I5"/>
+    <mergeCell ref="F6:I8"/>
+    <mergeCell ref="L59:R60"/>
+    <mergeCell ref="B59:I60"/>
     <mergeCell ref="F9:I11"/>
     <mergeCell ref="F12:I14"/>
     <mergeCell ref="J1:N1"/>
@@ -1020,8 +1203,6 @@
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A6:A8"/>
-    <mergeCell ref="F3:I5"/>
-    <mergeCell ref="F6:I8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>